<commit_message>
add annotation of cell types
</commit_message>
<xml_diff>
--- a/tables/methods-overview.xlsx
+++ b/tables/methods-overview.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\RandD\Units\IO Department\Bioinformatics\documentation\science\immune-signatures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\immune_deconvolution_benchmark\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9315" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>CIBERSORT</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE108901</t>
+  </si>
+  <si>
+    <t>EPIC</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +501,7 @@
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -517,8 +520,11 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,27 +547,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -580,13 +586,16 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -594,7 +603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -616,8 +625,11 @@
       <c r="G12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -636,13 +648,16 @@
       <c r="G13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -665,7 +680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -676,12 +691,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -700,11 +715,14 @@
       <c r="G18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -712,7 +730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="F22" s="1" t="s">
         <v>25</v>
       </c>
@@ -727,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add EPIC to Rscript and overview.
</commit_message>
<xml_diff>
--- a/tables/methods-overview.xlsx
+++ b/tables/methods-overview.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>CIBERSORT</t>
   </si>
@@ -121,6 +121,33 @@
   </si>
   <si>
     <t>EPIC</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Online + Sourcecode</t>
+  </si>
+  <si>
+    <t>Online + Sourcecode (old version)</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>bash pipeline/docker</t>
+  </si>
+  <si>
+    <t>Runs</t>
+  </si>
+  <si>
+    <t>Online + R package</t>
+  </si>
+  <si>
+    <t>https://github.com/GfellerLab/EPIC</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -484,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +525,7 @@
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -735,9 +762,60 @@
         <v>25</v>
       </c>
     </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update first spillover ananlysis, improve method overview table.
</commit_message>
<xml_diff>
--- a/tables/methods-overview.xlsx
+++ b/tables/methods-overview.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="9315"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>CIBERSORT</t>
   </si>
@@ -148,6 +149,15 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's the point of the different cancer types that can be specified? </t>
+  </si>
+  <si>
+    <t>x (online)</t>
+  </si>
+  <si>
+    <t>Linsley, Hoeck, Pabst, Becht, Tirosh</t>
   </si>
 </sst>
 </file>
@@ -171,15 +181,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,21 +203,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -511,309 +557,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H21" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B5:H14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Writing text and formatting gitbook.
</commit_message>
<xml_diff>
--- a/tables/methods-overview.xlsx
+++ b/tables/methods-overview.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="9315"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="method_overview" sheetId="1" r:id="rId1"/>
+    <sheet name="signatures" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="150">
   <si>
     <t>CIBERSORT</t>
   </si>
@@ -112,15 +111,6 @@
     <t>Linsley, Hoek, Beyer, De Simone (RNASeq)</t>
   </si>
   <si>
-    <t>datasets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ purified </t>
-  </si>
-  <si>
-    <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE108901</t>
-  </si>
-  <si>
     <t>EPIC</t>
   </si>
   <si>
@@ -158,13 +148,340 @@
   </si>
   <si>
     <t>Linsley, Hoeck, Pabst, Becht, Tirosh</t>
+  </si>
+  <si>
+    <t>B cells naive</t>
+  </si>
+  <si>
+    <t>B cells memory</t>
+  </si>
+  <si>
+    <t>Plasma cells</t>
+  </si>
+  <si>
+    <t>T cells CD8</t>
+  </si>
+  <si>
+    <t>T cells CD4 naive</t>
+  </si>
+  <si>
+    <t>T cells CD4 memory resting</t>
+  </si>
+  <si>
+    <t>T cells CD4 memory activated</t>
+  </si>
+  <si>
+    <t>T cells follicular helper</t>
+  </si>
+  <si>
+    <t>T cells regulatory (Tregs)</t>
+  </si>
+  <si>
+    <t>T cells gamma delta</t>
+  </si>
+  <si>
+    <t>NK cells resting</t>
+  </si>
+  <si>
+    <t>NK cells activated</t>
+  </si>
+  <si>
+    <t>Monocytes</t>
+  </si>
+  <si>
+    <t>Macrophages M0</t>
+  </si>
+  <si>
+    <t>Macrophages M1</t>
+  </si>
+  <si>
+    <t>Macrophages M2</t>
+  </si>
+  <si>
+    <t>Dendritic cells resting</t>
+  </si>
+  <si>
+    <t>Dendritic cells activated</t>
+  </si>
+  <si>
+    <t>Mast cells resting</t>
+  </si>
+  <si>
+    <t>Mast cells activated</t>
+  </si>
+  <si>
+    <t>Eosinophils</t>
+  </si>
+  <si>
+    <t>Neutrophils</t>
+  </si>
+  <si>
+    <t>B_cell</t>
+  </si>
+  <si>
+    <t>T_cell.CD4</t>
+  </si>
+  <si>
+    <t>T_cell.CD8</t>
+  </si>
+  <si>
+    <t>Neutrophil</t>
+  </si>
+  <si>
+    <t>Macrophage</t>
+  </si>
+  <si>
+    <t>does not sum to 1</t>
+  </si>
+  <si>
+    <t>sums to 1 in default mode</t>
+  </si>
+  <si>
+    <t>aDC</t>
+  </si>
+  <si>
+    <t>Adipocytes</t>
+  </si>
+  <si>
+    <t>Astrocytes</t>
+  </si>
+  <si>
+    <t>Basophils</t>
+  </si>
+  <si>
+    <t>B-cells</t>
+  </si>
+  <si>
+    <t>CD4+ memory T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ naive T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ Tcm</t>
+  </si>
+  <si>
+    <t>CD4+ Tem</t>
+  </si>
+  <si>
+    <t>CD8+ naive T-cells</t>
+  </si>
+  <si>
+    <t>CD8+ T-cells</t>
+  </si>
+  <si>
+    <t>CD8+ Tcm</t>
+  </si>
+  <si>
+    <t>CD8+ Tem</t>
+  </si>
+  <si>
+    <t>cDC</t>
+  </si>
+  <si>
+    <t>Chondrocytes</t>
+  </si>
+  <si>
+    <t>Class-switched memory B-cells</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>Endothelial cells</t>
+  </si>
+  <si>
+    <t>Epithelial cells</t>
+  </si>
+  <si>
+    <t>Erythrocytes</t>
+  </si>
+  <si>
+    <t>Fibroblasts</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Hepatocytes</t>
+  </si>
+  <si>
+    <t>HSC</t>
+  </si>
+  <si>
+    <t>iDC</t>
+  </si>
+  <si>
+    <t>Keratinocytes</t>
+  </si>
+  <si>
+    <t>ly Endothelial cells</t>
+  </si>
+  <si>
+    <t>Mast cells</t>
+  </si>
+  <si>
+    <t>Megakaryocytes</t>
+  </si>
+  <si>
+    <t>Melanocytes</t>
+  </si>
+  <si>
+    <t>Memory B-cells</t>
+  </si>
+  <si>
+    <t>MEP</t>
+  </si>
+  <si>
+    <t>Mesangial cells</t>
+  </si>
+  <si>
+    <t>MPP</t>
+  </si>
+  <si>
+    <t>MSC</t>
+  </si>
+  <si>
+    <t>mv Endothelial cells</t>
+  </si>
+  <si>
+    <t>Myocytes</t>
+  </si>
+  <si>
+    <t>naive B-cells</t>
+  </si>
+  <si>
+    <t>Neurons</t>
+  </si>
+  <si>
+    <t>NK cells</t>
+  </si>
+  <si>
+    <t>Osteoblast</t>
+  </si>
+  <si>
+    <t>pDC</t>
+  </si>
+  <si>
+    <t>Pericytes</t>
+  </si>
+  <si>
+    <t>Platelets</t>
+  </si>
+  <si>
+    <t>Preadipocytes</t>
+  </si>
+  <si>
+    <t>pro B-cells</t>
+  </si>
+  <si>
+    <t>Sebocytes</t>
+  </si>
+  <si>
+    <t>Skeletal muscle</t>
+  </si>
+  <si>
+    <t>Smooth muscle</t>
+  </si>
+  <si>
+    <t>Tgd cells</t>
+  </si>
+  <si>
+    <t>Th1 cells</t>
+  </si>
+  <si>
+    <t>Th2 cells</t>
+  </si>
+  <si>
+    <t>Tregs</t>
+  </si>
+  <si>
+    <t>ImmuneScore</t>
+  </si>
+  <si>
+    <t>StromaScore</t>
+  </si>
+  <si>
+    <t>MicroenvironmentScore</t>
+  </si>
+  <si>
+    <t>T cells</t>
+  </si>
+  <si>
+    <t>CD8 T cells</t>
+  </si>
+  <si>
+    <t>Cytotoxic lymphocytes</t>
+  </si>
+  <si>
+    <t>B lineage</t>
+  </si>
+  <si>
+    <t>Monocytic lineage</t>
+  </si>
+  <si>
+    <t>Myeloid dendritic cells</t>
+  </si>
+  <si>
+    <t>MCP counter</t>
+  </si>
+  <si>
+    <t>B.cells</t>
+  </si>
+  <si>
+    <t>Macrophages.M1</t>
+  </si>
+  <si>
+    <t>Macrophages.M2</t>
+  </si>
+  <si>
+    <t>NK.cells</t>
+  </si>
+  <si>
+    <t>T.cells.CD4</t>
+  </si>
+  <si>
+    <t>T.cells.CD8</t>
+  </si>
+  <si>
+    <t>Dendritic.cells</t>
+  </si>
+  <si>
+    <t>Bcells</t>
+  </si>
+  <si>
+    <t>CAFs</t>
+  </si>
+  <si>
+    <t>CD4_Tcells</t>
+  </si>
+  <si>
+    <t>CD8_Tcells</t>
+  </si>
+  <si>
+    <t>Endothelial</t>
+  </si>
+  <si>
+    <t>NKcells</t>
+  </si>
+  <si>
+    <t>otherCells</t>
+  </si>
+  <si>
+    <t>sums to 1 (has category "other")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +496,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -222,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -235,9 +565,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -261,7 +597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,13 +893,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
@@ -596,7 +932,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -622,7 +958,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -844,7 +1180,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -860,36 +1196,36 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="H19" t="s">
         <v>35</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -906,10 +1242,21 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -925,31 +1272,1233 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add preliminary validation study
</commit_message>
<xml_diff>
--- a/tables/methods-overview.xlsx
+++ b/tables/methods-overview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="method_overview" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
   <si>
     <t>CIBERSORT</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t>sums to 1 (has category "other")</t>
+  </si>
+  <si>
+    <t>according to correspondence paper, only comparison between samples of the same cancer type are feasible</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,6 +1262,11 @@
         <v>149</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B5:H14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1274,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>